<commit_message>
[2023-08-11] Major Updates on ROLODEX
</commit_message>
<xml_diff>
--- a/public/assets/files/ContactsCSVFileFormat.xlsx
+++ b/public/assets/files/ContactsCSVFileFormat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20112" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Salutation</t>
   </si>
@@ -37,6 +37,90 @@
   </si>
   <si>
     <t>Date of Birth</t>
+  </si>
+  <si>
+    <t>Office Phone</t>
+  </si>
+  <si>
+    <t>Mobile Phone</t>
+  </si>
+  <si>
+    <t>Home Phone</t>
+  </si>
+  <si>
+    <t>Secondary Phone</t>
+  </si>
+  <si>
+    <t>LinkedIn URL</t>
+  </si>
+  <si>
+    <t>Twitter URL</t>
+  </si>
+  <si>
+    <t>Instagram URL</t>
+  </si>
+  <si>
+    <t>Facebook URL</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Do Not Call</t>
+  </si>
+  <si>
+    <t>Lead Source</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Reports To</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Email OPT OUT</t>
+  </si>
+  <si>
+    <t>Mailing Street</t>
+  </si>
+  <si>
+    <t>Mailing PO Box</t>
+  </si>
+  <si>
+    <t>Mailing City</t>
+  </si>
+  <si>
+    <t>Mailing State</t>
+  </si>
+  <si>
+    <t>Mailing ZIP</t>
+  </si>
+  <si>
+    <t>Mailing Country</t>
+  </si>
+  <si>
+    <t>Other Street</t>
+  </si>
+  <si>
+    <t>Other PO Box</t>
+  </si>
+  <si>
+    <t>Other City</t>
+  </si>
+  <si>
+    <t>Other State</t>
+  </si>
+  <si>
+    <t>Other ZIP</t>
+  </si>
+  <si>
+    <t>Other Country</t>
+  </si>
+  <si>
+    <t>Decription</t>
   </si>
 </sst>
 </file>
@@ -66,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -89,13 +173,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,24 +495,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:AI1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -425,16 +524,100 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -448,7 +631,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -460,7 +643,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[2023-08-12] Contact Import Updates
</commit_message>
<xml_diff>
--- a/public/assets/files/ContactsCSVFileFormat.xlsx
+++ b/public/assets/files/ContactsCSVFileFormat.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\arkonorllc-crm\public\assets\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD8644B-F789-4F28-BDE4-F71C6242DD0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20112" windowHeight="8016"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Salutation</t>
   </si>
@@ -73,12 +77,6 @@
   </si>
   <si>
     <t>Department</t>
-  </si>
-  <si>
-    <t>Reports To</t>
-  </si>
-  <si>
-    <t>Assigned To</t>
   </si>
   <si>
     <t>Email OPT OUT</t>
@@ -126,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,6 +202,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -251,7 +252,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -284,9 +285,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -319,6 +337,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -494,26 +529,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AG1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" customWidth="1"/>
+    <col min="5" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,39 +647,9 @@
       </c>
       <c r="AG1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>